<commit_message>
Tweaking colorado gas model
</commit_message>
<xml_diff>
--- a/ColoradoModelSpecs.xlsx
+++ b/ColoradoModelSpecs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandt/PycharmProjects/SimulinkInterface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC5A969-0A46-504B-AD90-573624B92F30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FB163D-F14F-EA4B-A50A-5850B1C1CE43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="-19040" windowWidth="28800" windowHeight="15960" xr2:uid="{039CF851-ADCD-944A-A2B8-ED3DEEFF29CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{039CF851-ADCD-944A-A2B8-ED3DEEFF29CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>loadParm(4,:)</t>
   </si>
   <si>
-    <t>p: 6001, t: 7001, pt: 8001, tt: 9001</t>
-  </si>
-  <si>
     <t>Compressor: Denver Watkins</t>
   </si>
   <si>
@@ -107,12 +104,6 @@
     <t>PP: Colorado Springs</t>
   </si>
   <si>
-    <t>p: 6002, t: 7002, pt: 8002, tt: 9002</t>
-  </si>
-  <si>
-    <t>p: 6000, t: 7000, pt: 8000, tt: 9000</t>
-  </si>
-  <si>
     <t>loadParm(5,:)</t>
   </si>
   <si>
@@ -143,9 +134,6 @@
     <t>loadParm(7,:)</t>
   </si>
   <si>
-    <t>p: 6003, t: 7003, pt: 8003, tt: 9003</t>
-  </si>
-  <si>
     <t>Pipe: Cheyenne Wells to Springfield</t>
   </si>
   <si>
@@ -167,9 +155,6 @@
     <t>loadParm(9,:)</t>
   </si>
   <si>
-    <t>p: 6004, t: 7004, pt: 8004, tt: 9004</t>
-  </si>
-  <si>
     <t>Pipe: Cheyenne to Fort Morgan</t>
   </si>
   <si>
@@ -206,28 +191,43 @@
     <t>Modbus</t>
   </si>
   <si>
-    <t>5000, R:0</t>
-  </si>
-  <si>
-    <t>5001, R:0</t>
-  </si>
-  <si>
-    <t>5003, R:0</t>
-  </si>
-  <si>
-    <t>5004, R:0</t>
-  </si>
-  <si>
-    <t>5005, R:0</t>
-  </si>
-  <si>
-    <t>5006, R:0</t>
-  </si>
-  <si>
-    <t>5007, R:0</t>
-  </si>
-  <si>
     <t>Registers: 0,2,4,6 (respectively)</t>
+  </si>
+  <si>
+    <t>p: 8000, t: 9000</t>
+  </si>
+  <si>
+    <t>p: 8001, t: 9001</t>
+  </si>
+  <si>
+    <t>p: 8002, t: 9002</t>
+  </si>
+  <si>
+    <t>p: 8003, t: 9003</t>
+  </si>
+  <si>
+    <t>p: 8004, t: 9004</t>
+  </si>
+  <si>
+    <t>(5000, 0), p:(5100, 2), t:(5200, 4)</t>
+  </si>
+  <si>
+    <t>(5001, 0), p:(5101, 2), t:(5201, 4)</t>
+  </si>
+  <si>
+    <t>(5003, 0), p:(5103, 2), t:(5203, 4)</t>
+  </si>
+  <si>
+    <t>(5004, 0), p:(5104, 2), t:(5204, 4)</t>
+  </si>
+  <si>
+    <t>(5005, 0), p:(5105, 2), t:(5205, 4)</t>
+  </si>
+  <si>
+    <t>(5006, 0), p:(5106, 2), t:(5206, 4)</t>
+  </si>
+  <si>
+    <t>(5007, 0), p:(5107 , 2), t:(5207, 4)</t>
   </si>
 </sst>
 </file>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87B4C94-5961-6145-966D-2D9A2CE1BE69}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -615,7 +615,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>9090</v>
@@ -629,7 +629,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D3">
         <v>9091</v>
@@ -637,13 +637,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>9092</v>
@@ -651,13 +651,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>9093</v>
@@ -665,13 +665,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D6">
         <v>9094</v>
@@ -679,13 +679,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>9095</v>
@@ -693,13 +693,13 @@
     </row>
     <row r="8" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D8">
         <v>9096</v>
@@ -723,82 +723,82 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -809,13 +809,13 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D21">
         <v>9097</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -823,10 +823,10 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D22">
         <v>9098</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
@@ -842,13 +842,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="D24">
         <v>9099</v>
@@ -856,21 +856,21 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="D26">
         <v>10010</v>
@@ -878,21 +878,21 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D28">
         <v>10011</v>

</xml_diff>

<commit_message>
Adding experiment 1 code and colorado gas model.
</commit_message>
<xml_diff>
--- a/ColoradoModelSpecs.xlsx
+++ b/ColoradoModelSpecs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandt/PycharmProjects/SimulinkInterface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FB163D-F14F-EA4B-A50A-5850B1C1CE43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94E81B6-1836-4B45-8FDE-F13C5EC0F27E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{039CF851-ADCD-944A-A2B8-ED3DEEFF29CC}"/>
   </bookViews>
@@ -209,25 +209,25 @@
     <t>p: 8004, t: 9004</t>
   </si>
   <si>
-    <t>(5000, 0), p:(5100, 2), t:(5200, 4)</t>
-  </si>
-  <si>
-    <t>(5001, 0), p:(5101, 2), t:(5201, 4)</t>
-  </si>
-  <si>
-    <t>(5003, 0), p:(5103, 2), t:(5203, 4)</t>
-  </si>
-  <si>
-    <t>(5004, 0), p:(5104, 2), t:(5204, 4)</t>
-  </si>
-  <si>
-    <t>(5005, 0), p:(5105, 2), t:(5205, 4)</t>
-  </si>
-  <si>
-    <t>(5006, 0), p:(5106, 2), t:(5206, 4)</t>
-  </si>
-  <si>
-    <t>(5007, 0), p:(5107 , 2), t:(5207, 4)</t>
+    <t>(5000, 0), p:(5100, 2), t:(5200, 4), power_set: (6000)</t>
+  </si>
+  <si>
+    <t>(5001, 0), p:(5101, 2), t:(5201, 4), 6001</t>
+  </si>
+  <si>
+    <t>(5003, 0), p:(5103, 2), t:(5203, 4), 6003</t>
+  </si>
+  <si>
+    <t>(5004, 0), p:(5104, 2), t:(5204, 4), 6004</t>
+  </si>
+  <si>
+    <t>(5005, 0), p:(5105, 2), t:(5205, 4), 6005</t>
+  </si>
+  <si>
+    <t>(5006, 0), p:(5106, 2), t:(5206, 4), 6006</t>
+  </si>
+  <si>
+    <t>(5007, 0), p:(5107 , 2), t:(5207, 4), 6007</t>
   </si>
 </sst>
 </file>
@@ -582,14 +582,14 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="59.5" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Adding colorado gas model results and changes.
</commit_message>
<xml_diff>
--- a/ColoradoModelSpecs.xlsx
+++ b/ColoradoModelSpecs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandt/PycharmProjects/SimulinkInterface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94E81B6-1836-4B45-8FDE-F13C5EC0F27E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C44A2EB-22D9-D04B-944B-A1FE453A38A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{039CF851-ADCD-944A-A2B8-ED3DEEFF29CC}"/>
+    <workbookView xWindow="1300" yWindow="-16680" windowWidth="28800" windowHeight="15900" xr2:uid="{039CF851-ADCD-944A-A2B8-ED3DEEFF29CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87B4C94-5961-6145-966D-2D9A2CE1BE69}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>